<commit_message>
adding half of vendor info
</commit_message>
<xml_diff>
--- a/data/Vendor Information.xlsx
+++ b/data/Vendor Information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prash\DS4200\s-l-project-sbn2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B503A45-B934-4B37-AFEE-8A9A856132BF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6DD4A0-7436-432E-B6AE-2E4338736032}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DFAFABC8-D9E3-49EB-8929-D19649166CCC}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="121">
   <si>
     <t>Ackermann Maple Farm</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Commonwealth Kitchen</t>
   </si>
   <si>
-    <t>Consumers for Sensible Energy</t>
-  </si>
-  <si>
     <t>Crooked Stick Pop</t>
   </si>
   <si>
@@ -277,6 +274,126 @@
   </si>
   <si>
     <t>Zip Code</t>
+  </si>
+  <si>
+    <t>05647</t>
+  </si>
+  <si>
+    <t>02907</t>
+  </si>
+  <si>
+    <t>03304</t>
+  </si>
+  <si>
+    <t>02116</t>
+  </si>
+  <si>
+    <t>02467</t>
+  </si>
+  <si>
+    <t>01852</t>
+  </si>
+  <si>
+    <t>02139</t>
+  </si>
+  <si>
+    <t>01915</t>
+  </si>
+  <si>
+    <t>02675</t>
+  </si>
+  <si>
+    <t>02842</t>
+  </si>
+  <si>
+    <t>01230</t>
+  </si>
+  <si>
+    <t>02126</t>
+  </si>
+  <si>
+    <t>02136</t>
+  </si>
+  <si>
+    <t>02452</t>
+  </si>
+  <si>
+    <t>02129</t>
+  </si>
+  <si>
+    <t>01801</t>
+  </si>
+  <si>
+    <t>02120</t>
+  </si>
+  <si>
+    <t>02143</t>
+  </si>
+  <si>
+    <t>02576</t>
+  </si>
+  <si>
+    <t>02653</t>
+  </si>
+  <si>
+    <t>02121</t>
+  </si>
+  <si>
+    <t>01027</t>
+  </si>
+  <si>
+    <t>02111</t>
+  </si>
+  <si>
+    <t>02149</t>
+  </si>
+  <si>
+    <t>01776</t>
+  </si>
+  <si>
+    <t>04856</t>
+  </si>
+  <si>
+    <t>02906</t>
+  </si>
+  <si>
+    <t>02481</t>
+  </si>
+  <si>
+    <t>01375</t>
+  </si>
+  <si>
+    <t>01752</t>
+  </si>
+  <si>
+    <t>02109</t>
+  </si>
+  <si>
+    <t>03820</t>
+  </si>
+  <si>
+    <t>02823</t>
+  </si>
+  <si>
+    <t>02151</t>
+  </si>
+  <si>
+    <t>01035</t>
+  </si>
+  <si>
+    <t>02114</t>
+  </si>
+  <si>
+    <t>02461</t>
+  </si>
+  <si>
+    <t>02118</t>
+  </si>
+  <si>
+    <t>01984</t>
+  </si>
+  <si>
+    <t>02131</t>
   </si>
 </sst>
 </file>
@@ -312,8 +429,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,27 +746,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F38EF17-4F88-4442-A5D7-E5AE02A19D9E}">
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:C79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
         <v>79</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -658,6 +777,9 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -666,6 +788,9 @@
       <c r="B3" t="s">
         <v>1</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -674,6 +799,9 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -682,6 +810,9 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -690,6 +821,9 @@
       <c r="B6" t="s">
         <v>4</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -698,6 +832,9 @@
       <c r="B7" t="s">
         <v>5</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -706,6 +843,9 @@
       <c r="B8" t="s">
         <v>6</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -714,6 +854,9 @@
       <c r="B9" t="s">
         <v>7</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -722,6 +865,9 @@
       <c r="B10" t="s">
         <v>8</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -730,6 +876,9 @@
       <c r="B11" t="s">
         <v>9</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -738,6 +887,9 @@
       <c r="B12" t="s">
         <v>10</v>
       </c>
+      <c r="C12" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -746,6 +898,9 @@
       <c r="B13" t="s">
         <v>11</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -754,6 +909,9 @@
       <c r="B14" t="s">
         <v>12</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -762,6 +920,9 @@
       <c r="B15" t="s">
         <v>13</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -770,224 +931,308 @@
       <c r="B16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C39" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C41" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C42" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C43" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -995,7 +1240,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1003,7 +1248,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1011,7 +1256,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1019,7 +1264,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1273,14 +1518,6 @@
       </c>
       <c r="B79" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80">
-        <v>79</v>
-      </c>
-      <c r="B80" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completing vendor info for map; highlighting still needs to be fixed
</commit_message>
<xml_diff>
--- a/data/Vendor Information.xlsx
+++ b/data/Vendor Information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prash\DS4200\s-l-project-sbn2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6DD4A0-7436-432E-B6AE-2E4338736032}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B96F46-370A-4CEE-8CE7-22C445DD5371}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DFAFABC8-D9E3-49EB-8929-D19649166CCC}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="142">
   <si>
     <t>Ackermann Maple Farm</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Mr. Tamole</t>
   </si>
   <si>
-    <t>Mugger’s Marrow, LLC</t>
-  </si>
-  <si>
     <t>Dairy Promotion Board</t>
   </si>
   <si>
@@ -189,9 +186,6 @@
     <t>Our Family Farms</t>
   </si>
   <si>
-    <t>Painting as Art &amp; Ritual</t>
-  </si>
-  <si>
     <t>Prophecy Chocolate</t>
   </si>
   <si>
@@ -264,9 +258,6 @@
     <t>Waku</t>
   </si>
   <si>
-    <t>Wood Stove Kitchen</t>
-  </si>
-  <si>
     <t>Index</t>
   </si>
   <si>
@@ -394,6 +385,78 @@
   </si>
   <si>
     <t>02131</t>
+  </si>
+  <si>
+    <t>01742</t>
+  </si>
+  <si>
+    <t>02601</t>
+  </si>
+  <si>
+    <t>02138</t>
+  </si>
+  <si>
+    <t>02115</t>
+  </si>
+  <si>
+    <t>02113</t>
+  </si>
+  <si>
+    <t>01002</t>
+  </si>
+  <si>
+    <t>01702</t>
+  </si>
+  <si>
+    <t>01301</t>
+  </si>
+  <si>
+    <t>02457</t>
+  </si>
+  <si>
+    <t>02144</t>
+  </si>
+  <si>
+    <t>01331</t>
+  </si>
+  <si>
+    <t>01966</t>
+  </si>
+  <si>
+    <t>05482</t>
+  </si>
+  <si>
+    <t>05701</t>
+  </si>
+  <si>
+    <t>02885</t>
+  </si>
+  <si>
+    <t>02081</t>
+  </si>
+  <si>
+    <t>02356</t>
+  </si>
+  <si>
+    <t>02633</t>
+  </si>
+  <si>
+    <t>02110</t>
+  </si>
+  <si>
+    <t>01983</t>
+  </si>
+  <si>
+    <t>03263</t>
+  </si>
+  <si>
+    <t>02043</t>
+  </si>
+  <si>
+    <t>10956</t>
+  </si>
+  <si>
+    <t>20170</t>
   </si>
 </sst>
 </file>
@@ -746,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F38EF17-4F88-4442-A5D7-E5AE02A19D9E}">
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:C76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -761,13 +824,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -778,7 +841,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -789,7 +852,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -800,7 +863,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -811,7 +874,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -822,7 +885,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -833,7 +896,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -844,7 +907,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -855,7 +918,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -866,7 +929,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -877,7 +940,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -888,7 +951,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -899,7 +962,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -910,7 +973,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -921,7 +984,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -932,7 +995,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -943,7 +1006,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -954,7 +1017,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -965,7 +1028,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -976,7 +1039,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -987,7 +1050,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -998,7 +1061,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -1009,7 +1072,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1020,7 +1083,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -1031,7 +1094,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -1042,7 +1105,7 @@
         <v>24</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -1053,7 +1116,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -1064,7 +1127,7 @@
         <v>26</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1075,7 +1138,7 @@
         <v>27</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -1086,7 +1149,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1097,7 +1160,7 @@
         <v>29</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -1108,7 +1171,7 @@
         <v>30</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -1119,7 +1182,7 @@
         <v>31</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -1130,7 +1193,7 @@
         <v>32</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1141,7 +1204,7 @@
         <v>33</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1152,7 +1215,7 @@
         <v>34</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -1163,7 +1226,7 @@
         <v>35</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -1174,7 +1237,7 @@
         <v>36</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1185,7 +1248,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1196,7 +1259,7 @@
         <v>38</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1207,7 +1270,7 @@
         <v>39</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1218,7 +1281,7 @@
         <v>40</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -1229,7 +1292,7 @@
         <v>41</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -1239,6 +1302,9 @@
       <c r="B44" t="s">
         <v>42</v>
       </c>
+      <c r="C44" s="1" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
@@ -1247,6 +1313,9 @@
       <c r="B45" t="s">
         <v>43</v>
       </c>
+      <c r="C45" s="1" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
@@ -1255,6 +1324,9 @@
       <c r="B46" t="s">
         <v>44</v>
       </c>
+      <c r="C46" s="1" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
@@ -1263,6 +1335,9 @@
       <c r="B47" t="s">
         <v>45</v>
       </c>
+      <c r="C47" s="1" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
@@ -1271,253 +1346,316 @@
       <c r="B48" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C48" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C49" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C50" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C51" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C52" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C53" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C54" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C55" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C56" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C57" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C58" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C59" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C60" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C61" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C62" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C63" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C64" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C65" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C66" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C67" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C68" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C69" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C70" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C71" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C72" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C73" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C74" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C75" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77">
-        <v>76</v>
-      </c>
-      <c r="B77" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78">
-        <v>77</v>
-      </c>
-      <c r="B78" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79">
-        <v>78</v>
-      </c>
-      <c r="B79" t="s">
-        <v>77</v>
+      <c r="C76" s="1" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>